<commit_message>
update plant growth and ENA seuqncing templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/ENA/ENA_-_Raw_sequencing_reads.xlsx
+++ b/templates/dataplant/ENA/ENA_-_Raw_sequencing_reads.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.4</t>
+    <t>1.0.5</t>
   </si>
   <si>
     <t>Description</t>
@@ -179,15 +179,6 @@
     <t>Term Accession Number (DPBO:0000040)</t>
   </si>
   <si>
-    <t>Characteristic [Sequencing Library Name]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NCIT:C182058)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NCIT:C182058)</t>
-  </si>
-  <si>
     <t>Characteristic [Sequencing Library Source Indicator]</t>
   </si>
   <si>
@@ -224,16 +215,13 @@
     <t>Term Accession Number (DPBO:0000015)</t>
   </si>
   <si>
-    <t>Characteristic [MD5 Checksum]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NCIT:C171276)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NCIT:C171276)</t>
-  </si>
-  <si>
     <t>Output [Data]</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>Data Selector Format</t>
   </si>
   <si>
     <t/>
@@ -325,8 +313,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:W2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:W2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:S2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:S2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -346,35 +334,27 @@
     <filterColumn colId="16" hiddenButton="1"/>
     <filterColumn colId="17" hiddenButton="1"/>
     <filterColumn colId="18" hiddenButton="1"/>
-    <filterColumn colId="19" hiddenButton="1"/>
-    <filterColumn colId="20" hiddenButton="1"/>
-    <filterColumn colId="21" hiddenButton="1"/>
-    <filterColumn colId="22" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="23">
+  <tableColumns count="19">
     <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Component [next generation sequencing instrument model]" totalsRowFunction="none"/>
     <tableColumn id="3" name="Term Source REF (DPBO:0000040)" totalsRowFunction="none"/>
     <tableColumn id="4" name="Term Accession Number (DPBO:0000040)" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Characteristic [Sequencing Library Name]" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Term Source REF (NCIT:C182058)" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Term Accession Number (NCIT:C182058)" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Characteristic [Sequencing Library Source Indicator]" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Term Source REF (NCIT:C175895)" totalsRowFunction="none"/>
-    <tableColumn id="10" name="Term Accession Number (NCIT:C175895)" totalsRowFunction="none"/>
-    <tableColumn id="11" name="Parameter [Library selection]" totalsRowFunction="none"/>
-    <tableColumn id="12" name="Term Source REF (GENEPIO:0001940)" totalsRowFunction="none"/>
-    <tableColumn id="13" name="Term Accession Number (GENEPIO:0001940)" totalsRowFunction="none"/>
-    <tableColumn id="14" name="Parameter [library strategy]" totalsRowFunction="none"/>
-    <tableColumn id="15" name="Term Source REF (GENEPIO:0001973)" totalsRowFunction="none"/>
-    <tableColumn id="16" name="Term Accession Number (GENEPIO:0001973)" totalsRowFunction="none"/>
-    <tableColumn id="17" name="Parameter [library layout]" totalsRowFunction="none"/>
-    <tableColumn id="18" name="Term Source REF (DPBO:0000015)" totalsRowFunction="none"/>
-    <tableColumn id="19" name="Term Accession Number (DPBO:0000015)" totalsRowFunction="none"/>
-    <tableColumn id="20" name="Characteristic [MD5 Checksum]" totalsRowFunction="none"/>
-    <tableColumn id="21" name="Term Source REF (NCIT:C171276)" totalsRowFunction="none"/>
-    <tableColumn id="22" name="Term Accession Number (NCIT:C171276)" totalsRowFunction="none"/>
-    <tableColumn id="23" name="Output [Data]" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Characteristic [Sequencing Library Source Indicator]" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Term Source REF (NCIT:C175895)" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Term Accession Number (NCIT:C175895)" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Parameter [Library selection]" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Term Source REF (GENEPIO:0001940)" totalsRowFunction="none"/>
+    <tableColumn id="10" name="Term Accession Number (GENEPIO:0001940)" totalsRowFunction="none"/>
+    <tableColumn id="11" name="Parameter [library strategy]" totalsRowFunction="none"/>
+    <tableColumn id="12" name="Term Source REF (GENEPIO:0001973)" totalsRowFunction="none"/>
+    <tableColumn id="13" name="Term Accession Number (GENEPIO:0001973)" totalsRowFunction="none"/>
+    <tableColumn id="14" name="Parameter [library layout]" totalsRowFunction="none"/>
+    <tableColumn id="15" name="Term Source REF (DPBO:0000015)" totalsRowFunction="none"/>
+    <tableColumn id="16" name="Term Accession Number (DPBO:0000015)" totalsRowFunction="none"/>
+    <tableColumn id="17" name="Output [Data]" totalsRowFunction="none"/>
+    <tableColumn id="18" name="Data Format" totalsRowFunction="none"/>
+    <tableColumn id="19" name="Data Selector Format" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,10 +884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:S2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -965,88 +945,64 @@
       <c r="S1" t="s">
         <v>69</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>70</v>
       </c>
-      <c r="U1" t="s">
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="V1" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="W1" t="s">
+      <c r="D2" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
       </c>
       <c r="E2" t="s">
         <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" t="s">
         <v>78</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>79</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>80</v>
       </c>
-      <c r="L2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
         <v>81</v>
       </c>
-      <c r="N2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>83</v>
-      </c>
       <c r="Q2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="S2" t="s">
-        <v>85</v>
-      </c>
-      <c r="T2" t="s">
-        <v>74</v>
-      </c>
-      <c r="U2" t="s">
-        <v>74</v>
-      </c>
-      <c r="V2" t="s">
-        <v>74</v>
-      </c>
-      <c r="W2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverse changes to ENA raw sequencing reads
</commit_message>
<xml_diff>
--- a/templates/dataplant/ENA/ENA_-_Raw_sequencing_reads.xlsx
+++ b/templates/dataplant/ENA/ENA_-_Raw_sequencing_reads.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.5</t>
+    <t>1.0.4</t>
   </si>
   <si>
     <t>Description</t>
@@ -179,6 +179,15 @@
     <t>Term Accession Number (DPBO:0000040)</t>
   </si>
   <si>
+    <t>Characteristic [Sequencing Library Name]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C182058)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C182058)</t>
+  </si>
+  <si>
     <t>Characteristic [Sequencing Library Source Indicator]</t>
   </si>
   <si>
@@ -215,13 +224,16 @@
     <t>Term Accession Number (DPBO:0000015)</t>
   </si>
   <si>
+    <t>Characteristic [MD5 Checksum]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C171276)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C171276)</t>
+  </si>
+  <si>
     <t>Output [Data]</t>
-  </si>
-  <si>
-    <t>Data Format</t>
-  </si>
-  <si>
-    <t>Data Selector Format</t>
   </si>
   <si>
     <t/>
@@ -313,8 +325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:S2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:S2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:W2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:W2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -334,27 +346,35 @@
     <filterColumn colId="16" hiddenButton="1"/>
     <filterColumn colId="17" hiddenButton="1"/>
     <filterColumn colId="18" hiddenButton="1"/>
+    <filterColumn colId="19" hiddenButton="1"/>
+    <filterColumn colId="20" hiddenButton="1"/>
+    <filterColumn colId="21" hiddenButton="1"/>
+    <filterColumn colId="22" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="19">
+  <tableColumns count="23">
     <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Component [next generation sequencing instrument model]" totalsRowFunction="none"/>
     <tableColumn id="3" name="Term Source REF (DPBO:0000040)" totalsRowFunction="none"/>
     <tableColumn id="4" name="Term Accession Number (DPBO:0000040)" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Characteristic [Sequencing Library Source Indicator]" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Term Source REF (NCIT:C175895)" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Term Accession Number (NCIT:C175895)" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Parameter [Library selection]" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Term Source REF (GENEPIO:0001940)" totalsRowFunction="none"/>
-    <tableColumn id="10" name="Term Accession Number (GENEPIO:0001940)" totalsRowFunction="none"/>
-    <tableColumn id="11" name="Parameter [library strategy]" totalsRowFunction="none"/>
-    <tableColumn id="12" name="Term Source REF (GENEPIO:0001973)" totalsRowFunction="none"/>
-    <tableColumn id="13" name="Term Accession Number (GENEPIO:0001973)" totalsRowFunction="none"/>
-    <tableColumn id="14" name="Parameter [library layout]" totalsRowFunction="none"/>
-    <tableColumn id="15" name="Term Source REF (DPBO:0000015)" totalsRowFunction="none"/>
-    <tableColumn id="16" name="Term Accession Number (DPBO:0000015)" totalsRowFunction="none"/>
-    <tableColumn id="17" name="Output [Data]" totalsRowFunction="none"/>
-    <tableColumn id="18" name="Data Format" totalsRowFunction="none"/>
-    <tableColumn id="19" name="Data Selector Format" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Characteristic [Sequencing Library Name]" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Term Source REF (NCIT:C182058)" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Term Accession Number (NCIT:C182058)" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Characteristic [Sequencing Library Source Indicator]" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Term Source REF (NCIT:C175895)" totalsRowFunction="none"/>
+    <tableColumn id="10" name="Term Accession Number (NCIT:C175895)" totalsRowFunction="none"/>
+    <tableColumn id="11" name="Parameter [Library selection]" totalsRowFunction="none"/>
+    <tableColumn id="12" name="Term Source REF (GENEPIO:0001940)" totalsRowFunction="none"/>
+    <tableColumn id="13" name="Term Accession Number (GENEPIO:0001940)" totalsRowFunction="none"/>
+    <tableColumn id="14" name="Parameter [library strategy]" totalsRowFunction="none"/>
+    <tableColumn id="15" name="Term Source REF (GENEPIO:0001973)" totalsRowFunction="none"/>
+    <tableColumn id="16" name="Term Accession Number (GENEPIO:0001973)" totalsRowFunction="none"/>
+    <tableColumn id="17" name="Parameter [library layout]" totalsRowFunction="none"/>
+    <tableColumn id="18" name="Term Source REF (DPBO:0000015)" totalsRowFunction="none"/>
+    <tableColumn id="19" name="Term Accession Number (DPBO:0000015)" totalsRowFunction="none"/>
+    <tableColumn id="20" name="Characteristic [MD5 Checksum]" totalsRowFunction="none"/>
+    <tableColumn id="21" name="Term Source REF (NCIT:C171276)" totalsRowFunction="none"/>
+    <tableColumn id="22" name="Term Accession Number (NCIT:C171276)" totalsRowFunction="none"/>
+    <tableColumn id="23" name="Output [Data]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -884,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:W2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -945,64 +965,88 @@
       <c r="S1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
         <v>74</v>
       </c>
       <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s">
         <v>76</v>
       </c>
-      <c r="I2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>70</v>
-      </c>
       <c r="S2" t="s">
-        <v>70</v>
+        <v>85</v>
+      </c>
+      <c r="T2" t="s">
+        <v>74</v>
+      </c>
+      <c r="U2" t="s">
+        <v>74</v>
+      </c>
+      <c r="V2" t="s">
+        <v>74</v>
+      </c>
+      <c r="W2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>